<commit_message>
Chat de partida instalado, falla al dar ID al host
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\SO\SO_Project\Cliente\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D928DD1-6D02-4C46-9F94-962610198F16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{209E1E09-23E2-491D-BCAA-0C8C2169441D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Cliente</t>
   </si>
@@ -34,9 +28,6 @@
   </si>
   <si>
     <t>Registrarse</t>
-  </si>
-  <si>
-    <t>Login</t>
   </si>
   <si>
     <t>1$mensaje</t>
@@ -60,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -398,18 +389,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4623F32-CC7F-45DD-B406-4F5F6049AD81}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,7 +411,7 @@
     <col min="4" max="4" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -428,35 +419,29 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimizacion de nomenclaturas numericas
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>Registrarse</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Notificación</t>
   </si>
   <si>
-    <t>3$lista conectados actualizada</t>
-  </si>
-  <si>
     <t>Iniciar sesión</t>
   </si>
   <si>
@@ -63,36 +60,12 @@
     <t>Invitar jugadores</t>
   </si>
   <si>
-    <t>8/N/nombre1/…/nombreN</t>
-  </si>
-  <si>
-    <t>8$nombre_host/ID_partida</t>
-  </si>
-  <si>
-    <t>12$ID_partida</t>
-  </si>
-  <si>
     <t>Respuesta a invitación</t>
   </si>
   <si>
-    <t>9/ID_partida/respuesta</t>
-  </si>
-  <si>
-    <t>10$ID_partida/mensaje</t>
-  </si>
-  <si>
     <t>Mensaje en chat</t>
   </si>
   <si>
-    <t>10/ID_partida/mensaje</t>
-  </si>
-  <si>
-    <t>Salida de partida</t>
-  </si>
-  <si>
-    <t>11/ID_partida</t>
-  </si>
-  <si>
     <t>Observaciones</t>
   </si>
   <si>
@@ -124,6 +97,33 @@
   </si>
   <si>
     <t>Este mensaje se envía cuando un cliente quiere salir de una partida para que el servidor elimine sus datos de la lista de jugadores de la partida en cuestión.</t>
+  </si>
+  <si>
+    <t>4/N/nombre1/…/nombreN</t>
+  </si>
+  <si>
+    <t>5$nombre_host/ID_partida</t>
+  </si>
+  <si>
+    <t>4$ID_partida</t>
+  </si>
+  <si>
+    <t>5/ID_partida/respuesta</t>
+  </si>
+  <si>
+    <t>6$ID_partida/mensaje</t>
+  </si>
+  <si>
+    <t>6/ID_partida/mensaje</t>
+  </si>
+  <si>
+    <t>7/ID_partida</t>
+  </si>
+  <si>
+    <t>Solicitar lista de conectados</t>
+  </si>
+  <si>
+    <t>Salir de partida</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -496,7 +496,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +519,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -530,13 +530,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -547,112 +547,115 @@
         <v>3</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="B9" s="4" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Avances en el juego. No funciona aun
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Registrarse</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Este servicio se basa en intercambiar mensajes cuando los jugadores estan en una partida. Cuando un cliente envía uno, el servidor lo reenvía al resto de clientes.</t>
   </si>
   <si>
-    <t>Este mensaje se envía cuando un cliente quiere salir de una partida para que el servidor elimine sus datos de la lista de jugadores de la partida en cuestión.</t>
-  </si>
-  <si>
     <t>4/N/nombre1/…/nombreN</t>
   </si>
   <si>
@@ -124,6 +121,57 @@
   </si>
   <si>
     <t>Salir de partida</t>
+  </si>
+  <si>
+    <t>7$ID_partida</t>
+  </si>
+  <si>
+    <t>Configurar parámetros de partida</t>
+  </si>
+  <si>
+    <t>Comenzar partida</t>
+  </si>
+  <si>
+    <t>9/ID_partida</t>
+  </si>
+  <si>
+    <t>10/ID_partida/accion</t>
+  </si>
+  <si>
+    <t>9$ID_partida/estado/cartas/nombre</t>
+  </si>
+  <si>
+    <t>Este mensaje se envía cuando el host de una partida quiere que comienze la partida. En las respuestas del servidor se envía la fase en que se encuentra la ronda, las cartas que involucran al jugador y el nombre del dealer cuando comienza la ronda.</t>
+  </si>
+  <si>
+    <t>10$ID_partida/numJugador/accion</t>
+  </si>
+  <si>
+    <t>11$ID_partida/nombre</t>
+  </si>
+  <si>
+    <t>Esta notificación regula el turno de los jugadores para realizar acciones durante la partida</t>
+  </si>
+  <si>
+    <t>Establecer turnos</t>
+  </si>
+  <si>
+    <t>Transmitir acciones de jugadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cuando el jugador hace alguna acción, envía mensaje al servidor y este lo retransmite al resto de jugadores.</t>
+  </si>
+  <si>
+    <t>Este mensaje se envía cuando un cliente quiere salir de una partida para que el servidor elimine sus datos de la lista de jugadores de la partida en cuestión. En caso de que ese jugador sea el host de la partida, se designará al siguiente jugador en la lista como host.</t>
+  </si>
+  <si>
+    <t>8$ID_partida/numConfig/fichas/ciega/N/nombre1/…/nombreN</t>
+  </si>
+  <si>
+    <t>8/ID_partida/numConfig/fichas/ciega</t>
+  </si>
+  <si>
+    <t>Este mensaje se envía cuando el host de una partida quiere cambiar las fichas y la ciega mínima iniciales de una partida (numConfig = 0). Se reenvía el cambio al resto de jugadores de la partida. Además, cuando un jugador se une, se envía los parámetros y la lista de jugadores actualizada (numConfig = 2)</t>
   </si>
 </sst>
 </file>
@@ -159,11 +207,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -493,169 +538,237 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="91.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="57.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="91.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>25</v>
+      <c r="E9" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglo de errores i actualizacion de excel
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
   <si>
     <t>Registrarse</t>
   </si>
@@ -126,36 +126,9 @@
     <t>7$ID_partida</t>
   </si>
   <si>
-    <t>Configurar parámetros de partida</t>
-  </si>
-  <si>
     <t>Comenzar partida</t>
   </si>
   <si>
-    <t>9/ID_partida</t>
-  </si>
-  <si>
-    <t>10/ID_partida/accion</t>
-  </si>
-  <si>
-    <t>9$ID_partida/estado/cartas/nombre</t>
-  </si>
-  <si>
-    <t>Este mensaje se envía cuando el host de una partida quiere que comienze la partida. En las respuestas del servidor se envía la fase en que se encuentra la ronda, las cartas que involucran al jugador y el nombre del dealer cuando comienza la ronda.</t>
-  </si>
-  <si>
-    <t>10$ID_partida/numJugador/accion</t>
-  </si>
-  <si>
-    <t>11$ID_partida/nombre</t>
-  </si>
-  <si>
-    <t>Esta notificación regula el turno de los jugadores para realizar acciones durante la partida</t>
-  </si>
-  <si>
-    <t>Establecer turnos</t>
-  </si>
-  <si>
     <t>Transmitir acciones de jugadores</t>
   </si>
   <si>
@@ -165,13 +138,58 @@
     <t>Este mensaje se envía cuando un cliente quiere salir de una partida para que el servidor elimine sus datos de la lista de jugadores de la partida en cuestión. En caso de que ese jugador sea el host de la partida, se designará al siguiente jugador en la lista como host.</t>
   </si>
   <si>
-    <t>8$ID_partida/numConfig/fichas/ciega/N/nombre1/…/nombreN</t>
-  </si>
-  <si>
-    <t>8/ID_partida/numConfig/fichas/ciega</t>
-  </si>
-  <si>
-    <t>Este mensaje se envía cuando el host de una partida quiere cambiar las fichas y la ciega mínima iniciales de una partida (numConfig = 0). Se reenvía el cambio al resto de jugadores de la partida. Además, cuando un jugador se une, se envía los parámetros y la lista de jugadores actualizada (numConfig = 2)</t>
+    <t>12$ID_partida/N/nombre1/…/nombreN</t>
+  </si>
+  <si>
+    <t>13$ID_partida/numero1-palo1/numero2-palo2</t>
+  </si>
+  <si>
+    <t>14$ID_partida/numJugador/accion</t>
+  </si>
+  <si>
+    <t>Configurar lista de jugadores de la partida</t>
+  </si>
+  <si>
+    <t>12/ID_partida</t>
+  </si>
+  <si>
+    <t>13/ID_partida</t>
+  </si>
+  <si>
+    <t>14/ID_partida/accion</t>
+  </si>
+  <si>
+    <t>Darse de baja</t>
+  </si>
+  <si>
+    <t>RESERVADO CONSULTA 1 A BBDD</t>
+  </si>
+  <si>
+    <t>RESERVADO CONSULTA 2 A BBDD</t>
+  </si>
+  <si>
+    <t>8/clave</t>
+  </si>
+  <si>
+    <t>8$respuesta</t>
+  </si>
+  <si>
+    <t>Este mensaje se envía cuando un cliente quiere darse de baja de la base de datos del juego. Para ello, ha introducido su clave de acceso para verificar su identidad. Si la contraseña es incorrecta o hay algun problema con la base de datos se devuelve '-1' en la respuesta. Si todo ha ido bien, se elimina al jugador de la tabla y se devuelve 0.</t>
+  </si>
+  <si>
+    <t>Este mensaje se envía cuando un jugador se une a una partida para enviar la lista de jugadores actualizada a todos los jugadores de la partida. El jugador en cuestión pide al servidor que se la envíe exclusivamente a él una vez el entorno gráfico de la partida se ha cargado correctamente.</t>
+  </si>
+  <si>
+    <t>Este mensaje se envía cuando el host de una partida quiere que comienze la partida. En las respuestas del servidor se envía las dos cartas que cada jugador tiene inicialmente en la mano. Cda jugador recibe exclusivamente sus dos cartas, no recibe las del resto de jugadores.</t>
+  </si>
+  <si>
+    <t>9/nombre</t>
+  </si>
+  <si>
+    <t>9$respuesta</t>
+  </si>
+  <si>
+    <t>Este mensaje se envia cuando el cliente quiere recibir informacion sobre las partidas que ha jugado contra cierto jugador. Recibe el nombre, lo pasa por la base de datos buscando partidas en comun y devuelve la respuesta a la consulta. Devuelve 0/lista si todo ha ido bien (lista es la lista de ganadores de las partidas que han tenido en comun), -1 si no tenian partids en comun o -2 si hay algun error en la consulta a la base de datos.</t>
   </si>
 </sst>
 </file>
@@ -207,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -223,6 +241,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,9 +559,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -700,78 +721,106 @@
         <v>34</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
+      <c r="C15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C14:D14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Arreglando DOBLAR, aun no funciona
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arnau\Documents\UPC\2A\Sistemes Operatius\Poker_SO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B101E645-92BF-4C27-BCC5-344C4248681E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
   <si>
     <t>Registrarse</t>
   </si>
@@ -190,12 +196,15 @@
   </si>
   <si>
     <t>Este mensaje se envia cuando el cliente quiere recibir informacion sobre las partidas que ha jugado contra cierto jugador. Recibe el nombre, lo pasa por la base de datos buscando partidas en comun y devuelve la respuesta a la consulta. Devuelve 0/lista si todo ha ido bien (lista es la lista de ganadores de las partidas que han tenido en comun), -1 si no tenian partids en comun o -2 si hay algun error en la consulta a la base de datos.</t>
+  </si>
+  <si>
+    <t>Acciones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -551,18 +560,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +583,7 @@
     <col min="5" max="5" width="91.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
@@ -588,7 +597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -605,7 +614,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,7 +631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -639,7 +648,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -656,7 +665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -673,7 +682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -690,7 +699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -707,7 +716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -724,7 +733,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>46</v>
       </c>
@@ -741,7 +750,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
@@ -758,17 +767,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>42</v>
       </c>
@@ -783,7 +792,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -800,7 +809,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>36</v>
       </c>
@@ -815,6 +824,9 @@
       </c>
       <c r="E16" s="2" t="s">
         <v>37</v>
+      </c>
+      <c r="H16" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementacion de funcion para decidir ganador. Adaptacion total del juego al blackjack, falta probar
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arnau\Documents\UPC\2A\Sistemes Operatius\Poker_SO\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B101E645-92BF-4C27-BCC5-344C4248681E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -129,9 +123,6 @@
     <t>Salir de partida</t>
   </si>
   <si>
-    <t>7$ID_partida</t>
-  </si>
-  <si>
     <t>Comenzar partida</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t xml:space="preserve"> Cuando el jugador hace alguna acción, envía mensaje al servidor y este lo retransmite al resto de jugadores.</t>
   </si>
   <si>
-    <t>Este mensaje se envía cuando un cliente quiere salir de una partida para que el servidor elimine sus datos de la lista de jugadores de la partida en cuestión. En caso de que ese jugador sea el host de la partida, se designará al siguiente jugador en la lista como host.</t>
-  </si>
-  <si>
     <t>12$ID_partida/N/nombre1/…/nombreN</t>
   </si>
   <si>
@@ -199,12 +187,18 @@
   </si>
   <si>
     <t>Acciones</t>
+  </si>
+  <si>
+    <t>7$ID_partida/indexJugador</t>
+  </si>
+  <si>
+    <t>Este mensaje se envía cuando un cliente quiere salir de una partida para que el servidor elimine sus datos de la lista de jugadores de la partida en cuestión. Además, reenvia un mensaje con el inidce del jugador saliente al resto de jugadores para que lo tengan en cuenta.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -560,18 +554,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,106 +721,106 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="H16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Juego implementado, falta terminar partida
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Registrarse</t>
   </si>
@@ -193,6 +193,18 @@
   </si>
   <si>
     <t>Este mensaje se envía cuando un cliente quiere salir de una partida para que el servidor elimine sus datos de la lista de jugadores de la partida en cuestión. Además, reenvia un mensaje con el inidce del jugador saliente al resto de jugadores para que lo tengan en cuenta.</t>
+  </si>
+  <si>
+    <t>Pasar a siguiente ronda</t>
+  </si>
+  <si>
+    <t>15/ID_partida</t>
+  </si>
+  <si>
+    <t>15$ID_partida/indexJugador/fichas/puntos/numCartas/cartas</t>
+  </si>
+  <si>
+    <t>Cuando termina una ronda, el servidor envia notificaciones a los jugadores con las cartas, puntos y fichas de cada jugador y decide quien ha ganado la ronda. El cliente observa los resultados y responde pidiendo que comienze la siguiente.</t>
   </si>
 </sst>
 </file>
@@ -554,7 +566,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -562,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,6 +835,23 @@
         <v>55</v>
       </c>
     </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C14:D14"/>

</xml_diff>

<commit_message>
Implementado terminar partida. Funciona bien
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>Registrarse</t>
   </si>
@@ -186,9 +186,6 @@
     <t>Este mensaje se envia cuando el cliente quiere recibir informacion sobre las partidas que ha jugado contra cierto jugador. Recibe el nombre, lo pasa por la base de datos buscando partidas en comun y devuelve la respuesta a la consulta. Devuelve 0/lista si todo ha ido bien (lista es la lista de ganadores de las partidas que han tenido en comun), -1 si no tenian partids en comun o -2 si hay algun error en la consulta a la base de datos.</t>
   </si>
   <si>
-    <t>Acciones</t>
-  </si>
-  <si>
     <t>7$ID_partida/indexJugador</t>
   </si>
   <si>
@@ -205,6 +202,15 @@
   </si>
   <si>
     <t>Cuando termina una ronda, el servidor envia notificaciones a los jugadores con las cartas, puntos y fichas de cada jugador y decide quien ha ganado la ronda. El cliente observa los resultados y responde pidiendo que comienze la siguiente.</t>
+  </si>
+  <si>
+    <t>Terminar partida</t>
+  </si>
+  <si>
+    <t>16$ID_partida</t>
+  </si>
+  <si>
+    <t>Cuando el servidor detecta que una partida ha terminado, envia notificaciones a los jugadores</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -574,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,7 +595,7 @@
     <col min="5" max="5" width="91.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
@@ -603,7 +609,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -620,7 +626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -637,7 +643,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -654,7 +660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -671,7 +677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -688,7 +694,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -705,7 +711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -722,7 +728,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
@@ -733,13 +739,13 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>44</v>
       </c>
@@ -756,7 +762,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>45</v>
       </c>
@@ -773,17 +779,17 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -798,7 +804,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -815,7 +821,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
@@ -831,25 +837,39 @@
       <c r="E16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H16" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se ha añadido interfaz grafica a la cartas
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arnau\Documents\UPC\2A\Sistemes Operatius\Poker_SO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425C8FF5-C72D-47DA-97C6-CAB2BDACB08A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t>Registrarse</t>
   </si>
@@ -135,9 +141,6 @@
     <t>12$ID_partida/N/nombre1/…/nombreN</t>
   </si>
   <si>
-    <t>13$ID_partida/numero1-palo1/numero2-palo2</t>
-  </si>
-  <si>
     <t>14$ID_partida/numJugador/accion</t>
   </si>
   <si>
@@ -211,12 +214,27 @@
   </si>
   <si>
     <t>Cuando el servidor detecta que una partida ha terminado, envia notificaciones a los jugadores</t>
+  </si>
+  <si>
+    <t>13$ID_partida/puntos/numero1-palo1/numero2-palo2</t>
+  </si>
+  <si>
+    <t>Número palo</t>
+  </si>
+  <si>
+    <t>Carta</t>
+  </si>
+  <si>
+    <t>1. Picas
+2. Treboles
+3. Corazones
+4. Rombos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -246,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -265,6 +283,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -572,18 +593,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,6 +614,7 @@
     <col min="3" max="3" width="25.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="57.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="91.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -739,69 +761,69 @@
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>37</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -809,16 +831,16 @@
         <v>34</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -826,50 +848,63 @@
         <v>35</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="C17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>63</v>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+      <c r="G20" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="F21" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se han añadido las cartas de los otros jugadores
</commit_message>
<xml_diff>
--- a/ProtocoloClienteServidor.xlsx
+++ b/ProtocoloClienteServidor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arnau\Documents\UPC\2A\Sistemes Operatius\Poker_SO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B292D0-7A08-4C5A-A5F8-0C558008EA67}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C739853D-1932-47F9-BEF9-D78958C3F58D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -228,7 +228,7 @@
     <t>13$ID_partida/puntos/numero1-palo1/numero2-palo2/numJugador</t>
   </si>
   <si>
-    <t>Este mensaje se envía cuando el host de una partida quiere que comienze la partida. En las respuestas del servidor se envía las dos cartas que cada jugador tiene inicialmente en la mano. Cda jugador recibe exclusivamente sus dos cartas, no recibe las del resto de jugadores. Además, se recibe el identificador del jugador en la partida.</t>
+    <t>Este mensaje se envía cuando el host de una partida quiere que comienze la partida. En las respuestas del servidor se envía las dos cartas que cada jugador tiene inicialmente en la mano. Cda jugador recibe exclusivamente sus dos cartas, no recibe las del resto de jugadores. Además, se recibe el identificador del jugador en la partida, y el numero total de jugadores.</t>
   </si>
 </sst>
 </file>
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
     <col min="1" max="1" width="36.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" style="3" customWidth="1"/>
     <col min="3" max="3" width="25.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="65.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="82.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="91.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>

</xml_diff>